<commit_message>
updating sheet with email value
</commit_message>
<xml_diff>
--- a/score_sheet.xlsx
+++ b/score_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,6 +432,11 @@
           <t>29%</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>&lt;re.Match object; span=(8, 22), match='atest@test.com'&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -442,6 +447,45 @@
       <c r="B2" t="inlineStr">
         <is>
           <t>29%</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>&lt;re.Match object; span=(9, 23), match='atest@test.com'&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>resume_test.docx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>29%</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>atest@test.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>resume_test.pdf</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>29%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>atest@test.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
created function to handle unsupported files
</commit_message>
<xml_diff>
--- a/score_sheet.xlsx
+++ b/score_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,42 +446,64 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>resume_test - Copy - Copy (2).docx</t>
+          <t>resume_test - Copy - Copy - Copy.xyx</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>unsupported file (not a .pdf nor .docx</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>atest@test.com</t>
+          <t>unsupported file (not a .pdf nor .docx</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['+44123456789']</t>
+          <t>unsupported file (not a .pdf nor .docx</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>resume_test - Copy - Copy (2).docx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>atest@test.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['+44123456789']</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>resume_test - Copy - Copy (2).pdf</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>atest@test.com</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>['+44123456789']</t>
         </is>

</xml_diff>

<commit_message>
generated executable file, uploaded dummy files
</commit_message>
<xml_diff>
--- a/score_sheet.xlsx
+++ b/score_sheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>14%</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>14%</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>14%</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -534,73 +534,73 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>resume_test - Copy - Copy - Copy.docx</t>
+          <t>resume_test.odt</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>unsupported file (not a .pdf nor .docx</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>atest@test.com</t>
+          <t>unsupported file (not a .pdf nor .docx</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['+44123456789']</t>
+          <t>unsupported file (not a .pdf nor .docx</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>resume_test - Copy - Copy - Copy.xyx</t>
+          <t>resume_testr_randomwords (1).docx</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>unsupported file (not a .pdf nor .docx</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>unsupported file (not a .pdf nor .docx</t>
+          <t>eee@ttt.re</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>unsupported file (not a .pdf nor .docx</t>
+          <t>['+22000111222']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>resume_test - Copy - Copy (2).docx</t>
+          <t>resume_testr_randomwords (1).pdf</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>atest@test.com</t>
+          <t>gggggggg@g.uy</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['+44123456789']</t>
+          <t>['+11111111111111']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>resume_test - Copy - Copy (2).pdf</t>
+          <t>resume_testr_randomwords (2).docx</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -610,12 +610,56 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>atest@test.com</t>
+          <t>wow@indee.it</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['+44123456789']</t>
+          <t>['+55455253534']</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>resume_testr_randomwords.docx</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>xyz@zyx.com</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>['+478574123654']</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>resume_testr_randomwords.pdf</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>9%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>32@re.it</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>['+411111111111']</t>
         </is>
       </c>
     </row>

</xml_diff>